<commit_message>
investigate big datasets and flood hazard
</commit_message>
<xml_diff>
--- a/doc/indicator_search.xlsx
+++ b/doc/indicator_search.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devin\Desktop\CSU\Geospatial Centroid\NASA-prison-EJ\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccmothes\Desktop\NASA-prison-EJ\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABE3E82-30CF-4002-ADCA-C8F1730723CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24C82CF-1CCA-4A0B-82B7-3D6C04BABE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="2100" windowWidth="17280" windowHeight="9420" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
+    <workbookView xWindow="840" yWindow="3000" windowWidth="24030" windowHeight="12975" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
   <si>
     <t>indicator</t>
   </si>
@@ -167,9 +167,6 @@
     <t>https://gis.fema.gov/NFHL/NFHL_Key_Layers.gdb.zip</t>
   </si>
   <si>
-    <t xml:space="preserve">Full geodatabase </t>
-  </si>
-  <si>
     <t>Maybe</t>
   </si>
   <si>
@@ -324,6 +321,18 @@
   </si>
   <si>
     <t>Daily global Land Surface Temperature. Potentially more easy and efficient to work with.</t>
+  </si>
+  <si>
+    <t>USGS/GEE</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/earth-engine/datasets/catalog/USGS_NLCD_RELEASES_2016_REL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AK and HI are separate images, band for percent tree canopy cover. Code example of importing and mapping: https://code.earthengine.google.com/0530abe36a81b15ce425b3a11c81cefe </t>
+  </si>
+  <si>
+    <t>Full geodatabase; May also be able to pull map server with web services: https://hazards.fema.gov/femaportal/wps/portal/NFHLWMS</t>
   </si>
 </sst>
 </file>
@@ -686,25 +695,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E86D84-176C-47AA-8351-F9BBDD699BE6}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -733,17 +742,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -752,24 +761,24 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" t="s">
         <v>90</v>
       </c>
-      <c r="G3" t="s">
-        <v>91</v>
-      </c>
       <c r="H3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" t="s">
         <v>94</v>
       </c>
-      <c r="I3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
@@ -778,22 +787,22 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -822,121 +831,118 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="H6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>40</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>41</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="I8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>30</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>51</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -945,70 +951,76 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
         <v>46</v>
       </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
       <c r="G11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
         <v>48</v>
       </c>
-      <c r="H11" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" t="s">
         <v>53</v>
       </c>
-      <c r="I11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
         <v>71</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" t="s">
         <v>72</v>
       </c>
-      <c r="G12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I13" t="s">
         <v>73</v>
       </c>
-      <c r="I12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -1017,108 +1029,99 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H14" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
         <v>61</v>
       </c>
-      <c r="E15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G16" t="s">
         <v>62</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H16" t="s">
         <v>63</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I16" t="s">
         <v>64</v>
       </c>
-      <c r="I15" t="s">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" t="s">
         <v>69</v>
       </c>
-      <c r="H17" t="s">
-        <v>79</v>
-      </c>
-      <c r="I17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
@@ -1127,28 +1130,58 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" t="s">
         <v>81</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H19" t="s">
         <v>82</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I19" t="s">
         <v>83</v>
-      </c>
-      <c r="I18" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1" location="prods=149" xr:uid="{F264A2DB-1619-4E2C-84AD-32F894EAA961}"/>
+    <hyperlink ref="H9" r:id="rId1" location="prods=149" xr:uid="{F264A2DB-1619-4E2C-84AD-32F894EAA961}"/>
     <hyperlink ref="H4" r:id="rId2" location="description" xr:uid="{EECA4D4F-8922-4C5E-9EA6-1B7D81F7A1CA}"/>
+    <hyperlink ref="H8" r:id="rId3" xr:uid="{850225FF-2B8B-40C1-926B-9B3BD3033CD1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Buffer calculation function and point-data processing script
</commit_message>
<xml_diff>
--- a/doc/indicator_search.xlsx
+++ b/doc/indicator_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devin\Desktop\CSU\Geospatial Centroid\NASA-prison-EJ\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devin\Desktop\CSU\Geospatial Centroid\NASA-prison-EJ\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABE3E82-30CF-4002-ADCA-C8F1730723CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836685E-C8E4-4E9E-A8B3-51E1110E1E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="2100" windowWidth="17280" windowHeight="9420" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="100">
   <si>
     <t>indicator</t>
   </si>
@@ -324,6 +324,18 @@
   </si>
   <si>
     <t>Daily global Land Surface Temperature. Potentially more easy and efficient to work with.</t>
+  </si>
+  <si>
+    <t>National Risk Dataset</t>
+  </si>
+  <si>
+    <t>.csv, .shp, .gdb</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>https://hazards.fema.gov/nri/data-resources</t>
   </si>
 </sst>
 </file>
@@ -686,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E86D84-176C-47AA-8351-F9BBDD699BE6}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1145,6 +1157,32 @@
         <v>84</v>
       </c>
     </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H8" r:id="rId1" location="prods=149" xr:uid="{F264A2DB-1619-4E2C-84AD-32F894EAA961}"/>

</xml_diff>

<commit_message>
traffic density indicator details
</commit_message>
<xml_diff>
--- a/doc/indicator_search.xlsx
+++ b/doc/indicator_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccmothes\Desktop\NASA-prison-EJ\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246ADDE1-9AED-4411-B080-64E16C0CC207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E77B3A-BD8D-48E7-9B0E-9FA98577D834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27015" yWindow="1995" windowWidth="24030" windowHeight="12975" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
+    <workbookView xWindow="1095" yWindow="2760" windowWidth="24030" windowHeight="12975" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="107">
   <si>
     <t>indicator</t>
   </si>
@@ -345,6 +345,18 @@
   </si>
   <si>
     <t>Full geodatabase; May also be able to pull map server with web services: https://hazards.fema.gov/femaportal/wps/portal/NFHLWMS or investigate R package: https://github.com/mikejohnson51/NFHL</t>
+  </si>
+  <si>
+    <t>Use 2019 data</t>
+  </si>
+  <si>
+    <t>FHA</t>
+  </si>
+  <si>
+    <t>https://www.fhwa.dot.gov/policyinformation/hpms/shapefiles.cfm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methods from EJScreen and CO Enviroscreen: https://www.epa.gov/sites/default/files/2021-04/documents/ejscreen_technical_document.pdf </t>
   </si>
 </sst>
 </file>
@@ -707,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E86D84-176C-47AA-8351-F9BBDD699BE6}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,24 +1047,27 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>105</v>
+      </c>
+      <c r="I14" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1061,108 +1076,102 @@
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" t="s">
-        <v>57</v>
+        <v>75</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="I15" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>63</v>
+      </c>
+      <c r="I17" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
         <v>68</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -1171,47 +1180,76 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
         <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="H19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
         <v>96</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>46</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>97</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>41</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1219,6 +1257,7 @@
   <hyperlinks>
     <hyperlink ref="H9" r:id="rId1" location="prods=149" xr:uid="{F264A2DB-1619-4E2C-84AD-32F894EAA961}"/>
     <hyperlink ref="H4" r:id="rId2" location="description" xr:uid="{EECA4D4F-8922-4C5E-9EA6-1B7D81F7A1CA}"/>
+    <hyperlink ref="H15" r:id="rId3" xr:uid="{C77537AC-AD9D-42EA-9627-A1BB1909181E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
superfund, power_plants, init weight calculations
</commit_message>
<xml_diff>
--- a/doc/indicator_search.xlsx
+++ b/doc/indicator_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccmothes\Desktop\NASA-prison-EJ\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devin\Desktop\CSU\Geospatial Centroid\NASA-prison-EJ\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E77B3A-BD8D-48E7-9B0E-9FA98577D834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A3156E-4D8B-4F00-AF4F-1ADEB606BF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="2760" windowWidth="24030" windowHeight="12975" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -722,22 +722,22 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -774,7 +774,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -800,7 +800,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -826,7 +826,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -855,7 +855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -878,7 +878,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -901,7 +901,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -927,7 +927,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -950,7 +950,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -964,7 +964,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -990,7 +990,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
functionized pesticides and powerplants
</commit_message>
<xml_diff>
--- a/doc/indicator_search.xlsx
+++ b/doc/indicator_search.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devin\Desktop\CSU\Geospatial Centroid\NASA-prison-EJ\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A3156E-4D8B-4F00-AF4F-1ADEB606BF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086E30A0-730E-4F29-A24E-9FD531391131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="111">
   <si>
     <t>indicator</t>
   </si>
@@ -357,6 +357,18 @@
   </si>
   <si>
     <t xml:space="preserve">Methods from EJScreen and CO Enviroscreen: https://www.epa.gov/sites/default/files/2021-04/documents/ejscreen_technical_document.pdf </t>
+  </si>
+  <si>
+    <t>~200MB</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/ceam/303d-listed-impaired-waters</t>
+  </si>
+  <si>
+    <t>Impaired Waters (303d)</t>
+  </si>
+  <si>
+    <t>Segments, points</t>
   </si>
 </sst>
 </file>
@@ -711,7 +723,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -719,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E86D84-176C-47AA-8351-F9BBDD699BE6}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,6 +1265,32 @@
         <v>98</v>
       </c>
     </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H9" r:id="rId1" location="prods=149" xr:uid="{F264A2DB-1619-4E2C-84AD-32F894EAA961}"/>

</xml_diff>

<commit_message>
update RMP data source
</commit_message>
<xml_diff>
--- a/doc/indicator_search.xlsx
+++ b/doc/indicator_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devin\Desktop\CSU\Geospatial Centroid\NASA-prison-EJ\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccmothes\Desktop\NASA-prison-EJ\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086E30A0-730E-4F29-A24E-9FD531391131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43098CD4-BAD3-4D43-ABB6-79F2D6227D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
+    <workbookView xWindow="2715" yWindow="1470" windowWidth="21600" windowHeight="12735" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="116">
   <si>
     <t>indicator</t>
   </si>
@@ -369,13 +369,28 @@
   </si>
   <si>
     <t>Segments, points</t>
+  </si>
+  <si>
+    <t>Risk Management Plan (RMP)</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>1.8MB</t>
+  </si>
+  <si>
+    <t>https://hifld-geoplatform.opendata.arcgis.com/datasets/geoplatform::epa-emergency-response-er-risk-management-plan-rmp-facilities/explore?location=35.878600%2C-113.806709%2C3.92</t>
+  </si>
+  <si>
+    <t>Last Updated April 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +405,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF1B1B1B"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -413,9 +434,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -731,25 +753,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E86D84-176C-47AA-8351-F9BBDD699BE6}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -778,7 +800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -786,7 +808,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -812,7 +834,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -838,7 +860,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -867,7 +889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -890,7 +912,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -913,7 +935,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -939,7 +961,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -962,7 +984,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -976,7 +998,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1002,7 +1024,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1028,7 +1050,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1054,7 +1076,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1077,7 +1099,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1100,7 +1122,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1129,7 +1151,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1158,7 +1180,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -1181,7 +1203,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1210,7 +1232,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -1239,7 +1261,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -1265,7 +1287,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -1289,6 +1311,35 @@
       </c>
       <c r="H22" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I23" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1298,5 +1349,6 @@
     <hyperlink ref="H15" r:id="rId3" xr:uid="{C77537AC-AD9D-42EA-9627-A1BB1909181E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>